<commit_message>
updated the excel file with a few notes
</commit_message>
<xml_diff>
--- a/testSuite/aneoPuzzleAnalysis.xlsx
+++ b/testSuite/aneoPuzzleAnalysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\household\career\mezel\magnusine\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08EE5D99-AB5B-489A-93F6-27ED8C7D8897}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC79E78D-3550-4C12-BFF5-64309EAD173C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{C3F50968-A06E-47C6-B80E-666E5C5581C8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{C3F50968-A06E-47C6-B80E-666E5C5581C8}"/>
   </bookViews>
   <sheets>
     <sheet name="computations" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="120">
   <si>
     <t>maxSpeed</t>
   </si>
@@ -380,6 +380,12 @@
   </si>
   <si>
     <t>20300 30</t>
+  </si>
+  <si>
+    <t>The code to the right of this message is copy/pasted code of the test case file with the longest amount of lights on it (100). I verified knowing the correct intervals patterns using these cases</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The table to left of this message is reviewing a few of the test cases and seeing what condition various lights mapped to for a specific speed case. </t>
   </si>
 </sst>
 </file>
@@ -387,9 +393,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="177" formatCode="0.000000000000"/>
+    <numFmt numFmtId="164" formatCode="0.000000000000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -398,15 +411,20 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -414,22 +432,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="1" builtinId="10"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
-      <numFmt numFmtId="177" formatCode="0.000000000000"/>
+      <numFmt numFmtId="164" formatCode="0.000000000000"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -791,8 +829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE9795E0-966E-4AD6-937C-3AF609ED18CB}">
   <dimension ref="A1:T103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="F103" sqref="F103"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -813,13 +851,18 @@
         <v>130</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2">
         <v>6</v>
       </c>
+      <c r="O2" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
       <c r="R2" t="s">
         <v>18</v>
       </c>
@@ -854,6 +897,9 @@
       <c r="G3" t="s">
         <v>8</v>
       </c>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
       <c r="R3" t="s">
         <v>19</v>
       </c>
@@ -892,6 +938,9 @@
         <f>Table1[[#This Row],[timeToPassLight]]/Table1[[#This Row],[duration_h]]</f>
         <v>66</v>
       </c>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
       <c r="R4" t="s">
         <v>20</v>
       </c>
@@ -930,6 +979,9 @@
         <f>Table1[[#This Row],[timeToPassLight]]/Table1[[#This Row],[duration_h]]</f>
         <v>46</v>
       </c>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
       <c r="R5" t="s">
         <v>21</v>
       </c>
@@ -968,6 +1020,9 @@
         <f>Table1[[#This Row],[timeToPassLight]]/Table1[[#This Row],[duration_h]]</f>
         <v>35.999999999999993</v>
       </c>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
       <c r="R6" t="s">
         <v>22</v>
       </c>
@@ -1006,6 +1061,9 @@
         <f>Table1[[#This Row],[timeToPassLight]]/Table1[[#This Row],[duration_h]]</f>
         <v>30.000000000000004</v>
       </c>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
       <c r="R7" t="s">
         <v>23</v>
       </c>
@@ -1044,6 +1102,9 @@
         <f>Table1[[#This Row],[timeToPassLight]]/Table1[[#This Row],[duration_h]]</f>
         <v>26</v>
       </c>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="4"/>
       <c r="R8" t="s">
         <v>24</v>
       </c>
@@ -1082,6 +1143,9 @@
         <f>Table1[[#This Row],[timeToPassLight]]/Table1[[#This Row],[duration_h]]</f>
         <v>126.00000000000001</v>
       </c>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="4"/>
       <c r="R9" t="s">
         <v>25</v>
       </c>
@@ -4645,6 +4709,9 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="O2:Q9"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
@@ -4655,10 +4722,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC675D3E-35DB-4C78-94B2-208CE8B20DE0}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15:C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4668,7 +4735,7 @@
     <col min="3" max="3" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -4679,7 +4746,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4690,7 +4757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4701,7 +4768,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4712,7 +4779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4723,7 +4790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -4733,8 +4800,13 @@
       <c r="C8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E8" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3</v>
       </c>
@@ -4744,8 +4816,11 @@
       <c r="C9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>3</v>
       </c>
@@ -4755,8 +4830,11 @@
       <c r="C10">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>3</v>
       </c>
@@ -4766,8 +4844,11 @@
       <c r="C11">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>4</v>
       </c>
@@ -4777,8 +4858,11 @@
       <c r="C12">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>4</v>
       </c>
@@ -4788,8 +4872,11 @@
       <c r="C13">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>4</v>
       </c>
@@ -4799,8 +4886,11 @@
       <c r="C14">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>6</v>
       </c>
@@ -4811,7 +4901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>6</v>
       </c>
@@ -4845,6 +4935,9 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E8:G14"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="2">
     <tablePart r:id="rId1"/>

</xml_diff>